<commit_message>
Update Leave Card 6/29/2023 4:54 PM
</commit_message>
<xml_diff>
--- a/BELOSTRINO, JULIETA.xlsx
+++ b/BELOSTRINO, JULIETA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8931ADA4-0517-417A-BEFE-F023DBB8F20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -27,25 +28,17 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
   <si>
     <t>PERIOD</t>
   </si>
@@ -315,12 +308,15 @@
   </si>
   <si>
     <t>VL(3-0-0)</t>
+  </si>
+  <si>
+    <t>VL(1-0-0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -696,6 +692,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -728,9 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,7 +1248,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1295,7 +1291,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1355,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1419,7 +1415,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1481,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1548,7 +1544,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1646,7 +1642,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1705,7 +1701,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1770,7 +1766,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1813,7 +1809,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1888,7 +1884,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2074,7 +2070,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2140,7 +2136,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2198,7 +2194,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2264,7 +2260,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2316,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2395,7 +2391,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2438,7 +2434,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2504,7 +2500,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2560,7 +2556,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2639,7 +2635,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2656,25 +2652,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K135" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K135" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2686,25 +2682,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A8:K85" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table14" displayName="Table14" ref="A8:K84" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table14[EARNED])-SUM(Table14[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table14[[#This Row],[EARNED]]),"",Table14[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table14[[EARNED ]])-SUM(Table14[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3011,7 +3007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3021,7 +3017,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3029,95 +3025,95 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A82" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A31" activePane="bottomLeft"/>
       <selection activeCell="E9" sqref="E9"/>
-      <selection pane="bottomLeft" activeCell="L92" sqref="L92"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="52"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3125,7 +3121,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3138,24 +3134,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3214,7 +3210,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -3236,7 +3232,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3256,7 +3252,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3276,7 +3272,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3296,7 +3292,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3316,7 +3312,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3336,7 +3332,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3347,7 +3343,7 @@
       <c r="D16" s="43"/>
       <c r="E16" s="9"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="42">
+      <c r="G16" s="13">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
@@ -3356,7 +3352,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3376,7 +3372,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3396,7 +3392,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3416,7 +3412,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3436,7 +3432,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3456,7 +3452,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3480,7 +3476,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>47</v>
       </c>
@@ -3498,7 +3494,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3518,7 +3514,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3538,7 +3534,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3558,7 +3554,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3578,7 +3574,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3598,7 +3594,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3618,7 +3614,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3638,7 +3634,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3658,7 +3654,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3678,7 +3674,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3698,7 +3694,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="49"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3718,7 +3714,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3742,7 +3738,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>55</v>
       </c>
@@ -3760,7 +3756,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -3780,7 +3776,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="20" t="s">
         <v>61</v>
@@ -3800,7 +3796,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43862</v>
       </c>
@@ -3820,7 +3816,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43891</v>
       </c>
@@ -3840,7 +3836,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43922</v>
       </c>
@@ -3860,7 +3856,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43952</v>
       </c>
@@ -3880,7 +3876,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>43983</v>
       </c>
@@ -3900,7 +3896,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44013</v>
       </c>
@@ -3920,7 +3916,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -3936,7 +3932,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44044</v>
       </c>
@@ -3956,7 +3952,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44075</v>
       </c>
@@ -3976,7 +3972,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -3992,7 +3988,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40">
         <v>44105</v>
       </c>
@@ -4012,7 +4008,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44136</v>
       </c>
@@ -4032,7 +4028,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44166</v>
       </c>
@@ -4056,7 +4052,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
         <v>77</v>
       </c>
@@ -4074,7 +4070,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44197</v>
       </c>
@@ -4094,7 +4090,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44228</v>
       </c>
@@ -4120,7 +4116,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44256</v>
       </c>
@@ -4140,7 +4136,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44287</v>
       </c>
@@ -4160,7 +4156,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44317</v>
       </c>
@@ -4180,7 +4176,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44348</v>
       </c>
@@ -4206,7 +4202,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44378</v>
       </c>
@@ -4226,7 +4222,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44409</v>
       </c>
@@ -4246,7 +4242,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44440</v>
       </c>
@@ -4266,7 +4262,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40">
         <v>44470</v>
       </c>
@@ -4286,7 +4282,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44501</v>
       </c>
@@ -4306,7 +4302,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44531</v>
       </c>
@@ -4330,7 +4326,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="48" t="s">
         <v>80</v>
       </c>
@@ -4348,7 +4344,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>44562</v>
       </c>
@@ -4368,7 +4364,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44593</v>
       </c>
@@ -4388,7 +4384,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44621</v>
       </c>
@@ -4408,7 +4404,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
         <v>44652</v>
       </c>
@@ -4434,7 +4430,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
         <v>44682</v>
       </c>
@@ -4454,7 +4450,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44713</v>
       </c>
@@ -4474,7 +4470,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
         <v>44743</v>
       </c>
@@ -4500,7 +4496,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20" t="s">
         <v>51</v>
@@ -4522,7 +4518,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44774</v>
       </c>
@@ -4542,7 +4538,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40">
         <v>44805</v>
       </c>
@@ -4562,7 +4558,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40">
         <v>44835</v>
       </c>
@@ -4588,7 +4584,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20" t="s">
         <v>59</v>
@@ -4610,7 +4606,7 @@
         <v>44837</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40">
         <v>44866</v>
       </c>
@@ -4634,7 +4630,7 @@
         <v>44867</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20" t="s">
         <v>48</v>
@@ -4656,7 +4652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20" t="s">
         <v>59</v>
@@ -4678,7 +4674,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40">
         <v>44896</v>
       </c>
@@ -4704,7 +4700,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="23" t="s">
         <v>32</v>
       </c>
@@ -4728,7 +4724,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="23"/>
       <c r="B83" s="20" t="s">
         <v>46</v>
@@ -4748,7 +4744,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="48" t="s">
         <v>87</v>
       </c>
@@ -4766,7 +4762,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40">
         <v>44927</v>
       </c>
@@ -4792,7 +4788,7 @@
         <v>44957</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40">
         <v>44958</v>
       </c>
@@ -4812,7 +4808,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40">
         <v>44986</v>
       </c>
@@ -4838,7 +4834,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40">
         <v>45017</v>
       </c>
@@ -4858,7 +4854,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40">
         <v>45047</v>
       </c>
@@ -4878,8 +4874,8 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="61">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="40">
         <v>45078</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -4902,7 +4898,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4918,7 +4914,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4934,7 +4930,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4950,7 +4946,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4966,7 +4962,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4982,7 +4978,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4998,7 +4994,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -5014,7 +5010,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -5030,7 +5026,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -5046,7 +5042,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -5062,7 +5058,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -5078,7 +5074,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -5094,7 +5090,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -5110,7 +5106,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -5126,7 +5122,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -5142,7 +5138,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -5158,7 +5154,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -5174,7 +5170,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -5190,7 +5186,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5206,7 +5202,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5222,7 +5218,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5238,7 +5234,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5254,7 +5250,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5270,7 +5266,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5286,7 +5282,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5302,7 +5298,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5318,7 +5314,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5334,7 +5330,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5350,7 +5346,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5366,7 +5362,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5382,7 +5378,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5398,7 +5394,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5414,7 +5410,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5430,7 +5426,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5446,7 +5442,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5462,7 +5458,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5478,7 +5474,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5494,7 +5490,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5510,7 +5506,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5526,7 +5522,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5542,7 +5538,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5558,7 +5554,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5574,7 +5570,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5590,7 +5586,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -5606,14 +5602,14 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="41"/>
       <c r="B135" s="15"/>
       <c r="C135" s="42"/>
       <c r="D135" s="43"/>
       <c r="E135" s="9"/>
       <c r="F135" s="15"/>
-      <c r="G135" s="42" t="str">
+      <c r="G135" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
@@ -5637,10 +5633,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5663,95 +5659,95 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K85"/>
+  <dimension ref="A2:K84"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A28" activePane="bottomLeft"/>
-      <selection activeCell="I10" sqref="I10"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A43" activePane="bottomLeft"/>
+      <selection activeCell="I9" sqref="D9:I9"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="52"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -5759,7 +5755,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -5772,24 +5768,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -5824,7 +5820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -5833,7 +5829,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table14[EARNED])-SUM(Table14[Absence Undertime W/ Pay])+CONVERTION!A3</f>
-        <v>4.4170000000000016</v>
+        <v>3.4170000000000016</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -5848,7 +5844,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>47</v>
       </c>
@@ -5866,7 +5862,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43497</v>
       </c>
@@ -5890,7 +5886,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40"/>
       <c r="B12" s="20" t="s">
         <v>48</v>
@@ -5910,7 +5906,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43525</v>
       </c>
@@ -5934,7 +5930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43556</v>
       </c>
@@ -5958,7 +5954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="20" t="s">
         <v>48</v>
@@ -5980,7 +5976,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43586</v>
       </c>
@@ -6004,7 +6000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="20" t="s">
         <v>51</v>
@@ -6024,7 +6020,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43709</v>
       </c>
@@ -6048,7 +6044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40"/>
       <c r="B19" s="20" t="s">
         <v>48</v>
@@ -6070,7 +6066,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40"/>
       <c r="B20" s="20" t="s">
         <v>48</v>
@@ -6092,7 +6088,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43739</v>
       </c>
@@ -6116,7 +6112,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="48" t="s">
         <v>55</v>
       </c>
@@ -6134,7 +6130,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>43831</v>
       </c>
@@ -6158,7 +6154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="20" t="s">
         <v>61</v>
@@ -6178,7 +6174,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43862</v>
       </c>
@@ -6202,7 +6198,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43983</v>
       </c>
@@ -6226,7 +6222,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>44013</v>
       </c>
@@ -6250,7 +6246,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="20" t="s">
         <v>66</v>
@@ -6272,7 +6268,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>44044</v>
       </c>
@@ -6298,7 +6294,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>44075</v>
       </c>
@@ -6322,7 +6318,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="20" t="s">
         <v>73</v>
@@ -6346,7 +6342,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>44105</v>
       </c>
@@ -6370,7 +6366,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="48" t="s">
         <v>77</v>
       </c>
@@ -6388,7 +6384,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="48" t="s">
         <v>80</v>
       </c>
@@ -6403,7 +6399,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="20" t="s">
         <v>70</v>
@@ -6420,7 +6416,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>87</v>
       </c>
@@ -6435,8 +6431,10 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="40">
+        <v>45017</v>
+      </c>
       <c r="B37" s="20" t="s">
         <v>89</v>
       </c>
@@ -6446,19 +6444,26 @@
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="13" t="str">
+        <f>IF(ISBLANK(Table14[[#This Row],[EARNED]]),"",Table14[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
       <c r="H37" s="39"/>
       <c r="I37" s="9"/>
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
-        <v>45017</v>
-      </c>
-      <c r="B38" s="20"/>
+        <v>45097</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>90</v>
+      </c>
       <c r="C38" s="13"/>
-      <c r="D38" s="39"/>
+      <c r="D38" s="39">
+        <v>1</v>
+      </c>
       <c r="E38" s="9"/>
       <c r="F38" s="20"/>
       <c r="G38" s="13" t="str">
@@ -6468,9 +6473,11 @@
       <c r="H38" s="39"/>
       <c r="I38" s="9"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="50">
+        <v>45096</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -6484,8 +6491,9 @@
       <c r="H39" s="39"/>
       <c r="I39" s="9"/>
       <c r="J39" s="11"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="20"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -6501,7 +6509,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -6517,7 +6525,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -6533,7 +6541,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -6549,7 +6557,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -6565,7 +6573,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -6581,7 +6589,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -6597,7 +6605,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -6613,7 +6621,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -6629,7 +6637,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -6645,7 +6653,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -6661,7 +6669,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -6677,7 +6685,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -6693,7 +6701,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -6709,7 +6717,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -6725,7 +6733,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -6741,7 +6749,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -6757,7 +6765,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -6773,7 +6781,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -6789,7 +6797,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -6805,7 +6813,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -6821,7 +6829,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -6837,7 +6845,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -6853,7 +6861,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -6869,7 +6877,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -6885,7 +6893,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -6901,7 +6909,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -6917,7 +6925,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -6933,7 +6941,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -6949,7 +6957,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -6965,7 +6973,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -6981,7 +6989,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -6997,7 +7005,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -7013,7 +7021,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -7029,7 +7037,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -7045,7 +7053,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -7061,7 +7069,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -7077,7 +7085,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -7093,7 +7101,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -7109,7 +7117,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -7125,7 +7133,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -7141,7 +7149,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -7157,7 +7165,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -7173,7 +7181,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -7189,37 +7197,21 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="40"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="39"/>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="41"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="43"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="13" t="str">
+      <c r="F84" s="15"/>
+      <c r="G84" s="42" t="str">
         <f>IF(ISBLANK(Table14[[#This Row],[EARNED]]),"",Table14[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H84" s="39"/>
+      <c r="H84" s="43"/>
       <c r="I84" s="9"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="20"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="41"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="42" t="str">
-        <f>IF(ISBLANK(Table14[[#This Row],[EARNED]]),"",Table14[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H85" s="43"/>
-      <c r="I85" s="9"/>
-      <c r="J85" s="12"/>
-      <c r="K85" s="15"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7236,10 +7228,10 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7262,41 +7254,41 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="58" t="s">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="J1" s="59" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="J1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -7325,7 +7317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>43.417000000000002</v>
       </c>
@@ -7349,17 +7341,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -7373,14 +7365,14 @@
         <v>30</v>
       </c>
       <c r="G6" s="46"/>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -7407,7 +7399,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -7433,7 +7425,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -7459,7 +7451,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -7485,7 +7477,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -7511,7 +7503,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -7537,7 +7529,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -7563,7 +7555,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -7589,7 +7581,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -7609,7 +7601,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -7629,7 +7621,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -7649,7 +7641,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -7670,7 +7662,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -7691,7 +7683,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -7712,7 +7704,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -7733,7 +7725,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -7754,7 +7746,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -7775,7 +7767,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -7796,7 +7788,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -7817,7 +7809,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -7838,7 +7830,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -7859,7 +7851,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -7880,7 +7872,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -7901,7 +7893,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -7922,7 +7914,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -7943,7 +7935,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -7964,7 +7956,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -7985,7 +7977,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -8006,7 +7998,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -8027,7 +8019,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -8048,7 +8040,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -8069,7 +8061,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -8078,7 +8070,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -8087,7 +8079,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -8096,7 +8088,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -8105,7 +8097,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -8114,7 +8106,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -8123,7 +8115,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -8132,7 +8124,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -8141,7 +8133,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -8150,7 +8142,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -8159,7 +8151,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -8168,7 +8160,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -8177,7 +8169,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -8186,7 +8178,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -8195,7 +8187,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -8204,7 +8196,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -8213,7 +8205,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -8222,7 +8214,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -8231,7 +8223,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -8240,7 +8232,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -8249,7 +8241,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -8258,7 +8250,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -8267,7 +8259,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -8276,7 +8268,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -8285,7 +8277,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -8294,7 +8286,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -8303,7 +8295,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -8312,7 +8304,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -8321,7 +8313,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -8330,7 +8322,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>